<commit_message>
Add json meme file
</commit_message>
<xml_diff>
--- a/DankMemeStash.xlsx
+++ b/DankMemeStash.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,66 +27,150 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>Contempt</t>
-  </si>
-  <si>
-    <t>Disgust</t>
-  </si>
-  <si>
-    <t>Fear</t>
-  </si>
-  <si>
-    <t>Happiness</t>
-  </si>
-  <si>
-    <t>Anger</t>
-  </si>
-  <si>
-    <t>Neutral</t>
-  </si>
-  <si>
-    <t>Sadness</t>
-  </si>
-  <si>
-    <t>When a day-old meme is already stale and you lowkey miss being the center of attention</t>
-  </si>
-  <si>
-    <t>When you finally realize your winter body is just your regular body</t>
-  </si>
-  <si>
-    <t>When someone explains something to you three times and you still have no idea what's going on</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When you're about as ready for school as Mariah Carey was for the new year </t>
-  </si>
-  <si>
-    <t>When you retake a class after failing but fail it again</t>
-  </si>
-  <si>
-    <t>When you thought your meme was edgy but it gets removed</t>
-  </si>
-  <si>
-    <t>I am an ocean of emotion</t>
-  </si>
-  <si>
-    <t>When people say "Harambe was just a gorilla"</t>
-  </si>
-  <si>
-    <t>When you were supposed to start your paper at 8pm but now it's 2am and all you've done is look at memes</t>
-  </si>
-  <si>
-    <t>When you a 30 on the midterm and the median was a 28</t>
-  </si>
-  <si>
-    <t>When you find out you need a 425% on the final to pass with a C</t>
-  </si>
-  <si>
-    <t>When someone gets up to hand in their final but you're still flipping through the exam trying to find a problem you can actually solve</t>
-  </si>
-  <si>
-    <t>When you try to caffeinate yourself but you just end up increasing your heart rate while remaining exhausted</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+  <si>
+    <t>Sadness Top</t>
+  </si>
+  <si>
+    <t>Sadness Bottom</t>
+  </si>
+  <si>
+    <t>Happiness Top</t>
+  </si>
+  <si>
+    <t>Happiness Bottom</t>
+  </si>
+  <si>
+    <t>Contempt Top</t>
+  </si>
+  <si>
+    <t>Contempt Bottom</t>
+  </si>
+  <si>
+    <t>Fear Top</t>
+  </si>
+  <si>
+    <t>Fear Bottom</t>
+  </si>
+  <si>
+    <t>Neutral Top</t>
+  </si>
+  <si>
+    <t>Neutral Bottom</t>
+  </si>
+  <si>
+    <t>When you're on a diet</t>
+  </si>
+  <si>
+    <t>and people keep bringing junk food to work</t>
+  </si>
+  <si>
+    <t>I didn't choose the thug life</t>
+  </si>
+  <si>
+    <t>The thug life chose me</t>
+  </si>
+  <si>
+    <t>you wake up and the charger wasn't plugged in</t>
+  </si>
+  <si>
+    <t>How you look when</t>
+  </si>
+  <si>
+    <t>When you hold the door for someone</t>
+  </si>
+  <si>
+    <t>and ten people walk through</t>
+  </si>
+  <si>
+    <t>Disgust Top</t>
+  </si>
+  <si>
+    <t>Disgust Bottom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> is just your regular body</t>
+  </si>
+  <si>
+    <t>When you finally realize your winter body</t>
+  </si>
+  <si>
+    <t>and you still have no idea what's going on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When someone explains something to you three times </t>
+  </si>
+  <si>
+    <t xml:space="preserve">as Mariah Carey was for the new year </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you're about as ready for school </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> and the median was a 28</t>
+  </si>
+  <si>
+    <t>When you get a 30 on the midterm</t>
+  </si>
+  <si>
+    <t>and you lowkey miss being the center of attention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When a day-old meme is already stale </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Harambe was just a gorilla"</t>
+  </si>
+  <si>
+    <t>Anger Top</t>
+  </si>
+  <si>
+    <t>Anger Bottom</t>
+  </si>
+  <si>
+    <t>When people say</t>
+  </si>
+  <si>
+    <t>When you thought your meme was edgy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> but then it gets removed</t>
+  </si>
+  <si>
+    <t>but you're still flipping through the exam trying to find a problem you can actually solve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When someone gets up to hand in their final </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> to pass with a C</t>
+  </si>
+  <si>
+    <t>When you find out you need a 425% on the final</t>
+  </si>
+  <si>
+    <t>but fail it again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you retake a class after failing </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> of emotion</t>
+  </si>
+  <si>
+    <t>I am an ocean</t>
+  </si>
+  <si>
+    <t>but now it's 2am and all you've done is look at memes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you were supposed to start your paper at 8pm </t>
+  </si>
+  <si>
+    <t>but you just end up increasing your heart rate while remaining exhausted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When you try to caffeinate yourself </t>
   </si>
 </sst>
 </file>
@@ -130,10 +214,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,85 +494,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane xSplit="11" ySplit="18" topLeftCell="L19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>